<commit_message>
Add data.xlsx for test data
</commit_message>
<xml_diff>
--- a/data.xlsx
+++ b/data.xlsx
@@ -81,13 +81,19 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
     </font>
     <font>
       <u/>
@@ -124,12 +130,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
     </xf>
-    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="1" applyFont="1" fillId="0" applyAlignment="1">
+    <xf xfId="0" numFmtId="0" borderId="1" applyBorder="1" fontId="2" applyFont="1" fillId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
@@ -443,87 +455,87 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="2" max="2" style="3" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="1" max="1" style="4" width="13.576428571428572" customWidth="1" bestFit="1"/>
+    <col min="2" max="2" style="5" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
     <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="2" customHeight="1" ht="19.5">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="3" customHeight="1" ht="19.5">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B3" s="2" t="s">
         <v>5</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="4" customHeight="1" ht="19.5">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="1" t="s">
+      <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="5" customHeight="1" ht="19.5">
-      <c r="A5" s="2" t="s">
+      <c r="A5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="6" customHeight="1" ht="19.5">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="B6" s="1" t="s">
+      <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="7" customHeight="1" ht="19.5">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="1" t="s">
+      <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="8" customHeight="1" ht="19.5">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B8" s="1" t="s">
+      <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="9" customHeight="1" ht="18.75">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>17</v>
       </c>
     </row>
     <row x14ac:dyDescent="0.25" r="10" customHeight="1" ht="18.75">
-      <c r="A10" s="2" t="s">
+      <c r="A10" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B10" s="1" t="s">
+      <c r="B10" s="2" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>